<commit_message>
Data Validation full update
</commit_message>
<xml_diff>
--- a/Videos/VideoLaps.xlsx
+++ b/Videos/VideoLaps.xlsx
@@ -1,26 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\OneDrive\Documents\Cycling\Aero tests\Body Rocket\Tests\Newport_010722\Cleaned\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\OneDrive\Documents\Cycling\Aero tests\Body Rocket\Tests\Newport_010722\Videos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{C44DB5F8-98E3-4438-A617-89E97E056275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2312F229-C0D9-4F97-8AB0-2C2D6846B7F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="VideoLaps" sheetId="1" r:id="rId1"/>
+    <sheet name="Settings" sheetId="2" r:id="rId1"/>
+    <sheet name="VideoLaps" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" iterate="1"/>
+  <definedNames>
+    <definedName name="Videos_Folder">Settings!$B$1</definedName>
+  </definedNames>
+  <calcPr calcId="191029" iterate="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="37">
   <si>
     <t>Test-Run</t>
   </si>
@@ -49,9 +65,6 @@
     <t>Distance (m)</t>
   </si>
   <si>
-    <t>R4</t>
-  </si>
-  <si>
     <t>Grd-Speed</t>
   </si>
   <si>
@@ -67,44 +80,80 @@
     <t>Crk-Speed</t>
   </si>
   <si>
-    <t>R6</t>
-  </si>
-  <si>
-    <t>R7</t>
-  </si>
-  <si>
-    <t>R8</t>
-  </si>
-  <si>
     <t>Vid_crk_angle</t>
   </si>
   <si>
     <t>?</t>
   </si>
   <si>
-    <t>Crank_Revs</t>
+    <t>Changed gear at some point</t>
   </si>
   <si>
-    <t>sw_speed</t>
+    <t>R04</t>
   </si>
   <si>
-    <t>sw_time</t>
+    <t>R06</t>
   </si>
   <si>
-    <t>br_time</t>
+    <t>R07</t>
   </si>
   <si>
-    <t>Changed gear at some point</t>
+    <t>R08</t>
+  </si>
+  <si>
+    <t>Frame</t>
+  </si>
+  <si>
+    <t>Vid_FWh_ang</t>
+  </si>
+  <si>
+    <t>Vid_RWh_ang</t>
+  </si>
+  <si>
+    <t>BR_Dist</t>
+  </si>
+  <si>
+    <t>BR_Time</t>
+  </si>
+  <si>
+    <t>Vid_Wh_Dist</t>
+  </si>
+  <si>
+    <t>Vid_Crk_Dist</t>
+  </si>
+  <si>
+    <t>Vid_Wh_Speed</t>
+  </si>
+  <si>
+    <t>Vid_Crk_revs</t>
+  </si>
+  <si>
+    <t>Vid_Wh_revs</t>
+  </si>
+  <si>
+    <t>Vid_Durtn</t>
+  </si>
+  <si>
+    <t>Vid_Time</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>C:\Users\user\OneDrive\Documents\Cycling\Aero tests\Body Rocket\Tests\Newport_010722\Videos</t>
+  </si>
+  <si>
+    <t>Videos folder</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.000"/>
-  </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,8 +289,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="5" tint="-0.249977111117893"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -249,13 +306,58 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -441,6 +543,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -558,7 +666,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -601,19 +709,69 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="42" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -647,6 +805,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -966,25 +1125,62 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X57"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5673CCD-C7DC-4852-8689-B888C489A8C1}">
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="2.7265625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="5.36328125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="12.90625" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Y57"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="U20" sqref="U20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15" style="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5703125" style="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" style="12"/>
+    <col min="17" max="17" width="9.140625" style="19"/>
+    <col min="18" max="18" width="9.140625" style="18"/>
+    <col min="19" max="19" width="12.5703125" style="19" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.140625" style="18"/>
+    <col min="23" max="23" width="12.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.7109375" style="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1012,25 +1208,55 @@
       <c r="I1" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="K1" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="O1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="R1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="P1" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q1" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="R1" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="S1" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="T1" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="U1" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="V1" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="W1" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="X1" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B2">
         <v>4</v>
@@ -1056,13 +1282,17 @@
       <c r="I2">
         <v>28.234999999999999</v>
       </c>
-      <c r="L2" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="K2" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE(Videos_Folder,"\",A2,"-Lap",TEXT(B2,"00"),".MOV"),CONCATENATE(A2,"-Lap",TEXT(B2,"00"),".MOV"))</f>
+        <v>R04-Lap04.MOV</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B3">
         <v>6</v>
@@ -1088,13 +1318,17 @@
       <c r="I3">
         <v>221.315</v>
       </c>
-      <c r="L3" s="3">
+      <c r="K3" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE(Videos_Folder,"\",A3,"-Lap",TEXT(B3,"00"),".MOV"),CONCATENATE(A3,"-Lap",TEXT(B3,"00"),".MOV"))</f>
+        <v>R04-Lap06.MOV</v>
+      </c>
+      <c r="M3" s="9">
         <v>231</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B4">
         <v>8</v>
@@ -1120,13 +1354,17 @@
       <c r="I4">
         <v>103.33499999999999</v>
       </c>
-      <c r="L4" s="3">
+      <c r="K4" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE(Videos_Folder,"\",A4,"-Lap",TEXT(B4,"00"),".MOV"),CONCATENATE(A4,"-Lap",TEXT(B4,"00"),".MOV"))</f>
+        <v>R04-Lap08.MOV</v>
+      </c>
+      <c r="M4" s="9">
         <v>110</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B5">
         <v>10</v>
@@ -1152,10 +1390,15 @@
       <c r="I5">
         <v>15.36</v>
       </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="K5" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE(Videos_Folder,"\",A5,"-Lap",TEXT(B5,"00"),".MOV"),CONCATENATE(A5,"-Lap",TEXT(B5,"00"),".MOV"))</f>
+        <v>R04-Lap10.MOV</v>
+      </c>
+      <c r="M5" s="9"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B6">
         <v>12</v>
@@ -1181,10 +1424,15 @@
       <c r="I6">
         <v>206.32</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="K6" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE(Videos_Folder,"\",A6,"-Lap",TEXT(B6,"00"),".MOV"),CONCATENATE(A6,"-Lap",TEXT(B6,"00"),".MOV"))</f>
+        <v>R04-Lap12.MOV</v>
+      </c>
+      <c r="M6" s="9"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B7">
         <v>14</v>
@@ -1210,10 +1458,15 @@
       <c r="I7">
         <v>56.47</v>
       </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="K7" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE(Videos_Folder,"\",A7,"-Lap",TEXT(B7,"00"),".MOV"),CONCATENATE(A7,"-Lap",TEXT(B7,"00"),".MOV"))</f>
+        <v>R04-Lap14.MOV</v>
+      </c>
+      <c r="M7" s="9"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B8">
         <v>16</v>
@@ -1239,10 +1492,15 @@
       <c r="I8">
         <v>304.33</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="K8" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE(Videos_Folder,"\",A8,"-Lap",TEXT(B8,"00"),".MOV"),CONCATENATE(A8,"-Lap",TEXT(B8,"00"),".MOV"))</f>
+        <v>R04-Lap16.MOV</v>
+      </c>
+      <c r="M8" s="9"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B9">
         <v>18</v>
@@ -1268,10 +1526,15 @@
       <c r="I9">
         <v>119.49</v>
       </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="K9" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE(Videos_Folder,"\",A9,"-Lap",TEXT(B9,"00"),".MOV"),CONCATENATE(A9,"-Lap",TEXT(B9,"00"),".MOV"))</f>
+        <v>R04-Lap18.MOV</v>
+      </c>
+      <c r="M9" s="9"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B10">
         <v>20</v>
@@ -1297,155 +1560,235 @@
       <c r="I10">
         <v>41.805</v>
       </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="K10" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE(Videos_Folder,"\",A10,"-Lap",TEXT(B10,"00"),".MOV"),CONCATENATE(A10,"-Lap",TEXT(B10,"00"),".MOV"))</f>
+        <v>R04-Lap20.MOV</v>
+      </c>
+      <c r="M10" s="9"/>
+    </row>
+    <row r="11" spans="1:25" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="7">
+        <v>20</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0</v>
+      </c>
+      <c r="D11" s="7">
+        <v>0</v>
+      </c>
+      <c r="E11" s="7">
+        <v>0</v>
+      </c>
+      <c r="F11" s="7">
+        <v>0</v>
+      </c>
+      <c r="G11" s="7">
+        <v>0</v>
+      </c>
+      <c r="H11" s="7">
+        <v>12.117754609779</v>
+      </c>
+      <c r="I11" s="7">
+        <v>0</v>
+      </c>
+      <c r="J11" s="13"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="20"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="20"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2"/>
+    </row>
+    <row r="12" spans="1:25" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="B12" s="7">
         <v>20</v>
       </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>12.1610154738896</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="C12" s="7">
+        <v>0</v>
+      </c>
+      <c r="D12" s="7">
+        <v>0</v>
+      </c>
+      <c r="E12" s="7">
+        <v>0</v>
+      </c>
+      <c r="F12" s="7">
+        <v>0</v>
+      </c>
+      <c r="G12" s="7">
+        <v>0</v>
+      </c>
+      <c r="H12" s="7">
+        <v>11.954589944253801</v>
+      </c>
+      <c r="I12" s="7">
+        <v>0</v>
+      </c>
+      <c r="J12" s="13"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="20"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="20"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
+    </row>
+    <row r="13" spans="1:25" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="B13" s="7">
         <v>20</v>
       </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>11.988508220503</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="C13" s="7">
+        <v>0</v>
+      </c>
+      <c r="D13" s="7">
+        <v>0</v>
+      </c>
+      <c r="E13" s="7">
+        <v>0</v>
+      </c>
+      <c r="F13" s="7">
+        <v>0</v>
+      </c>
+      <c r="G13" s="7">
+        <v>0</v>
+      </c>
+      <c r="H13" s="7">
+        <v>12.1153372909541</v>
+      </c>
+      <c r="I13" s="7">
+        <v>0</v>
+      </c>
+      <c r="J13" s="13"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="20"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="20"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2"/>
+    </row>
+    <row r="14" spans="1:25" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B13">
+      <c r="B14" s="7">
         <v>20</v>
       </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>12.157848464702001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="C14" s="7">
+        <v>0</v>
+      </c>
+      <c r="D14" s="7">
+        <v>0</v>
+      </c>
+      <c r="E14" s="7">
+        <v>0</v>
+      </c>
+      <c r="F14" s="7">
+        <v>0</v>
+      </c>
+      <c r="G14" s="7">
+        <v>0</v>
+      </c>
+      <c r="H14" s="7">
+        <v>11.954677298311401</v>
+      </c>
+      <c r="I14" s="7">
+        <v>0</v>
+      </c>
+      <c r="J14" s="13"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="20"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="20"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+    </row>
+    <row r="15" spans="1:25" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B14">
+      <c r="B15" s="7">
         <v>20</v>
       </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>11.9884795091877</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>20</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>12.173667533683499</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="C15" s="7">
+        <v>0</v>
+      </c>
+      <c r="D15" s="7">
+        <v>0</v>
+      </c>
+      <c r="E15" s="7">
+        <v>0</v>
+      </c>
+      <c r="F15" s="7">
+        <v>0</v>
+      </c>
+      <c r="G15" s="7">
+        <v>0</v>
+      </c>
+      <c r="H15" s="7">
+        <v>12.1317673678713</v>
+      </c>
+      <c r="I15" s="7">
+        <v>0</v>
+      </c>
+      <c r="J15" s="13"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="20"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+      <c r="V15" s="20"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -1471,10 +1814,15 @@
       <c r="I16">
         <v>56.034999999999997</v>
       </c>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="K16" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE(Videos_Folder,"\",A16,"-Lap",TEXT(B16,"00"),".MOV"),CONCATENATE(A16,"-Lap",TEXT(B16,"00"),".MOV"))</f>
+        <v>R06-Lap04.MOV</v>
+      </c>
+      <c r="M16" s="9"/>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B17">
         <v>6</v>
@@ -1500,10 +1848,15 @@
       <c r="I17">
         <v>65.14</v>
       </c>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="K17" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE(Videos_Folder,"\",A17,"-Lap",TEXT(B17,"00"),".MOV"),CONCATENATE(A17,"-Lap",TEXT(B17,"00"),".MOV"))</f>
+        <v>R06-Lap06.MOV</v>
+      </c>
+      <c r="M17" s="9"/>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B18">
         <v>8</v>
@@ -1529,10 +1882,15 @@
       <c r="I18">
         <v>115.795</v>
       </c>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="K18" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE(Videos_Folder,"\",A18,"-Lap",TEXT(B18,"00"),".MOV"),CONCATENATE(A18,"-Lap",TEXT(B18,"00"),".MOV"))</f>
+        <v>R06-Lap08.MOV</v>
+      </c>
+      <c r="M18" s="9"/>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B19">
         <v>10</v>
@@ -1558,10 +1916,15 @@
       <c r="I19">
         <v>141.30000000000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="K19" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE(Videos_Folder,"\",A19,"-Lap",TEXT(B19,"00"),".MOV"),CONCATENATE(A19,"-Lap",TEXT(B19,"00"),".MOV"))</f>
+        <v>R06-Lap10.MOV</v>
+      </c>
+      <c r="M19" s="9"/>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>12</v>
@@ -1587,10 +1950,15 @@
       <c r="I20">
         <v>174.26</v>
       </c>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="K20" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE(Videos_Folder,"\",A20,"-Lap",TEXT(B20,"00"),".MOV"),CONCATENATE(A20,"-Lap",TEXT(B20,"00"),".MOV"))</f>
+        <v>R06-Lap12.MOV</v>
+      </c>
+      <c r="M20" s="9"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B21">
         <v>14</v>
@@ -1616,10 +1984,15 @@
       <c r="I21">
         <v>154.55000000000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="K21" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE(Videos_Folder,"\",A21,"-Lap",TEXT(B21,"00"),".MOV"),CONCATENATE(A21,"-Lap",TEXT(B21,"00"),".MOV"))</f>
+        <v>R06-Lap14.MOV</v>
+      </c>
+      <c r="M21" s="9"/>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B22">
         <v>16</v>
@@ -1645,10 +2018,15 @@
       <c r="I22">
         <v>63.02</v>
       </c>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="K22" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE(Videos_Folder,"\",A22,"-Lap",TEXT(B22,"00"),".MOV"),CONCATENATE(A22,"-Lap",TEXT(B22,"00"),".MOV"))</f>
+        <v>R06-Lap16.MOV</v>
+      </c>
+      <c r="M22" s="9"/>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B23">
         <v>18</v>
@@ -1674,10 +2052,15 @@
       <c r="I23">
         <v>55.72</v>
       </c>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="K23" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE(Videos_Folder,"\",A23,"-Lap",TEXT(B23,"00"),".MOV"),CONCATENATE(A23,"-Lap",TEXT(B23,"00"),".MOV"))</f>
+        <v>R06-Lap18.MOV</v>
+      </c>
+      <c r="M23" s="9"/>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B24">
         <v>20</v>
@@ -1703,155 +2086,235 @@
       <c r="I24">
         <v>145.04499999999999</v>
       </c>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+      <c r="K24" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE(Videos_Folder,"\",A24,"-Lap",TEXT(B24,"00"),".MOV"),CONCATENATE(A24,"-Lap",TEXT(B24,"00"),".MOV"))</f>
+        <v>R06-Lap20.MOV</v>
+      </c>
+      <c r="M24" s="9"/>
+    </row>
+    <row r="25" spans="1:24" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="7">
+        <v>20</v>
+      </c>
+      <c r="C25" s="7">
+        <v>0</v>
+      </c>
+      <c r="D25" s="7">
+        <v>0</v>
+      </c>
+      <c r="E25" s="7">
+        <v>0</v>
+      </c>
+      <c r="F25" s="7">
+        <v>0</v>
+      </c>
+      <c r="G25" s="7">
+        <v>0</v>
+      </c>
+      <c r="H25" s="7">
+        <v>11.822107213838001</v>
+      </c>
+      <c r="I25" s="7">
+        <v>0</v>
+      </c>
+      <c r="J25" s="13"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="20"/>
+      <c r="S25" s="2"/>
+      <c r="T25" s="2"/>
+      <c r="U25" s="2"/>
+      <c r="V25" s="20"/>
+      <c r="W25" s="2"/>
+      <c r="X25" s="2"/>
+    </row>
+    <row r="26" spans="1:24" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B25">
+      <c r="B26" s="7">
         <v>20</v>
       </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-      <c r="G25">
-        <v>0</v>
-      </c>
-      <c r="H25">
-        <v>0</v>
-      </c>
-      <c r="I25">
-        <v>11.8997483940056</v>
-      </c>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+      <c r="C26" s="7">
+        <v>0</v>
+      </c>
+      <c r="D26" s="7">
+        <v>0</v>
+      </c>
+      <c r="E26" s="7">
+        <v>0</v>
+      </c>
+      <c r="F26" s="7">
+        <v>0</v>
+      </c>
+      <c r="G26" s="7">
+        <v>0</v>
+      </c>
+      <c r="H26" s="7">
+        <v>11.567391631304501</v>
+      </c>
+      <c r="I26" s="7">
+        <v>0</v>
+      </c>
+      <c r="J26" s="13"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="8"/>
+      <c r="P26" s="8"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="20"/>
+      <c r="S26" s="2"/>
+      <c r="T26" s="2"/>
+      <c r="U26" s="2"/>
+      <c r="V26" s="20"/>
+      <c r="W26" s="2"/>
+      <c r="X26" s="2"/>
+    </row>
+    <row r="27" spans="1:24" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B26">
+      <c r="B27" s="7">
         <v>20</v>
       </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-      <c r="G26">
-        <v>0</v>
-      </c>
-      <c r="H26">
-        <v>0</v>
-      </c>
-      <c r="I26">
-        <v>11.6390738758029</v>
-      </c>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+      <c r="C27" s="7">
+        <v>0</v>
+      </c>
+      <c r="D27" s="7">
+        <v>0</v>
+      </c>
+      <c r="E27" s="7">
+        <v>0</v>
+      </c>
+      <c r="F27" s="7">
+        <v>0</v>
+      </c>
+      <c r="G27" s="7">
+        <v>0</v>
+      </c>
+      <c r="H27" s="7">
+        <v>11.8198230112275</v>
+      </c>
+      <c r="I27" s="7">
+        <v>0</v>
+      </c>
+      <c r="J27" s="13"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="8"/>
+      <c r="P27" s="8"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="20"/>
+      <c r="S27" s="2"/>
+      <c r="T27" s="2"/>
+      <c r="U27" s="2"/>
+      <c r="V27" s="20"/>
+      <c r="W27" s="2"/>
+      <c r="X27" s="2"/>
+    </row>
+    <row r="28" spans="1:24" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B27">
+      <c r="B28" s="7">
         <v>20</v>
       </c>
-      <c r="C27">
-        <v>0</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
-      <c r="G27">
-        <v>0</v>
-      </c>
-      <c r="H27">
-        <v>0</v>
-      </c>
-      <c r="I27">
-        <v>11.897027420891099</v>
-      </c>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+      <c r="C28" s="7">
+        <v>0</v>
+      </c>
+      <c r="D28" s="7">
+        <v>0</v>
+      </c>
+      <c r="E28" s="7">
+        <v>0</v>
+      </c>
+      <c r="F28" s="7">
+        <v>0</v>
+      </c>
+      <c r="G28" s="7">
+        <v>0</v>
+      </c>
+      <c r="H28" s="7">
+        <v>11.567486212576799</v>
+      </c>
+      <c r="I28" s="7">
+        <v>0</v>
+      </c>
+      <c r="J28" s="13"/>
+      <c r="K28" s="16"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="8"/>
+      <c r="O28" s="8"/>
+      <c r="P28" s="8"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="20"/>
+      <c r="S28" s="2"/>
+      <c r="T28" s="2"/>
+      <c r="U28" s="2"/>
+      <c r="V28" s="20"/>
+      <c r="W28" s="2"/>
+      <c r="X28" s="2"/>
+    </row>
+    <row r="29" spans="1:24" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B28">
+      <c r="B29" s="7">
         <v>20</v>
       </c>
-      <c r="C28">
-        <v>0</v>
-      </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
-      <c r="H28">
-        <v>0</v>
-      </c>
-      <c r="I28">
-        <v>11.6390425489728</v>
-      </c>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29">
-        <v>20</v>
-      </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-      <c r="G29">
-        <v>0</v>
-      </c>
-      <c r="H29">
-        <v>0</v>
-      </c>
-      <c r="I29">
-        <v>11.9138590315071</v>
-      </c>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="C29" s="7">
+        <v>0</v>
+      </c>
+      <c r="D29" s="7">
+        <v>0</v>
+      </c>
+      <c r="E29" s="7">
+        <v>0</v>
+      </c>
+      <c r="F29" s="7">
+        <v>0</v>
+      </c>
+      <c r="G29" s="7">
+        <v>0</v>
+      </c>
+      <c r="H29" s="7">
+        <v>11.8369152274045</v>
+      </c>
+      <c r="I29" s="7">
+        <v>0</v>
+      </c>
+      <c r="J29" s="13"/>
+      <c r="K29" s="16"/>
+      <c r="L29" s="16"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="8"/>
+      <c r="O29" s="8"/>
+      <c r="P29" s="8"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="20"/>
+      <c r="S29" s="2"/>
+      <c r="T29" s="2"/>
+      <c r="U29" s="2"/>
+      <c r="V29" s="20"/>
+      <c r="W29" s="2"/>
+      <c r="X29" s="2"/>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B30">
         <v>4</v>
@@ -1874,28 +2337,32 @@
       <c r="H30">
         <v>496.98</v>
       </c>
-      <c r="I30" s="6">
+      <c r="I30" s="4">
         <v>160.99</v>
       </c>
-      <c r="K30" s="2">
+      <c r="K30" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE(Videos_Folder,"\",A30,"-Lap",TEXT(B30,"00"),".MOV"),CONCATENATE(A30,"-Lap",TEXT(B30,"00"),".MOV"))</f>
+        <v>R07-Lap04.MOV</v>
+      </c>
+      <c r="L30" s="15">
         <v>502</v>
       </c>
-      <c r="L30" s="3">
-        <v>160.99</v>
-      </c>
-      <c r="M30">
+      <c r="M30" s="9">
+        <v>195</v>
+      </c>
+      <c r="N30" s="8">
         <v>294</v>
       </c>
-      <c r="N30">
+      <c r="O30" s="12">
         <v>72</v>
       </c>
-      <c r="O30">
+      <c r="P30" s="12">
         <v>10.96</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B31">
         <v>6</v>
@@ -1918,57 +2385,64 @@
       <c r="H31">
         <v>747.73</v>
       </c>
-      <c r="I31" s="6">
+      <c r="I31" s="4">
         <v>181.905</v>
       </c>
-      <c r="L31" s="3">
-        <v>181.905</v>
-      </c>
-      <c r="M31">
+      <c r="K31" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE(Videos_Folder,"\",A31,"-Lap",TEXT(B31,"00"),".MOV"),CONCATENATE(A31,"-Lap",TEXT(B31,"00"),".MOV"))</f>
+        <v>R07-Lap06.MOV</v>
+      </c>
+      <c r="L31" s="15">
+        <v>423</v>
+      </c>
+      <c r="M31" s="9">
+        <v>63</v>
+      </c>
+      <c r="N31" s="8">
         <v>236</v>
       </c>
-      <c r="N31">
+      <c r="O31" s="12">
         <v>98</v>
       </c>
-      <c r="O31">
+      <c r="P31" s="12">
         <v>32.619999999999997</v>
       </c>
-      <c r="P31">
-        <f>O31-O30</f>
+      <c r="Q31" s="19">
+        <f>P31-P30</f>
         <v>21.659999999999997</v>
       </c>
-      <c r="Q31">
+      <c r="R31" s="21">
         <f>G31-G30</f>
         <v>21.615000000000002</v>
       </c>
-      <c r="R31" s="4">
-        <f>ROUNDDOWN(250/((E31/F31)*(D31/1000)),0)+(IF(L31&gt;L30,(L31-L30)/360,(L31+360-L30)/360))</f>
-        <v>33.058097222222223</v>
-      </c>
-      <c r="S31">
-        <f>ROUNDDOWN(R31*(E31/F31),0)+IF(M31&gt;M30,(M31-M30)/360,(M31+360-M30)/360)</f>
-        <v>118.83888888888889</v>
-      </c>
-      <c r="T31">
-        <f>S31*(D31/1000)</f>
-        <v>249.08631111111112</v>
-      </c>
-      <c r="U31">
+      <c r="S31" s="22">
+        <f>ROUNDDOWN(250/((E31/F31)*(D31/1000)),0)+(IF(M31&gt;M30,(M31-M30)/360,(M31+360-M30)/360))</f>
+        <v>33.633333333333333</v>
+      </c>
+      <c r="T31" s="22">
+        <f>ROUNDDOWN(S31*(E31/F31),0)+IF(N31&gt;N30,(N31-N30)/360,(N31+360-N30)/360)</f>
+        <v>120.83888888888889</v>
+      </c>
+      <c r="U31" s="22">
+        <f>T31*(D31/1000)</f>
+        <v>253.27831111111112</v>
+      </c>
+      <c r="V31" s="21">
         <f>H31-H30</f>
         <v>250.75</v>
       </c>
-      <c r="V31">
-        <f>T31/P31</f>
-        <v>11.499829691187033</v>
-      </c>
-      <c r="W31">
-        <f>R31*(E30/F30)*(D30/1000)</f>
-        <v>247.46347063492067</v>
-      </c>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="W31" s="22">
+        <f>S31*(E30/F30)*(D30/1000)</f>
+        <v>251.76952380952383</v>
+      </c>
+      <c r="X31" s="22">
+        <f>U31/Q31</f>
+        <v>11.693366163947884</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B32">
         <v>8</v>
@@ -1991,57 +2465,64 @@
       <c r="H32">
         <v>998.42</v>
       </c>
-      <c r="I32" s="6">
+      <c r="I32" s="4">
         <v>200.065</v>
       </c>
-      <c r="K32" s="2">
-        <v>238</v>
-      </c>
-      <c r="L32" s="3">
-        <v>200.065</v>
-      </c>
-      <c r="M32">
-        <v>144</v>
-      </c>
-      <c r="O32">
+      <c r="K32" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE(Videos_Folder,"\",A32,"-Lap",TEXT(B32,"00"),".MOV"),CONCATENATE(A32,"-Lap",TEXT(B32,"00"),".MOV"))</f>
+        <v>R07-Lap08.MOV</v>
+      </c>
+      <c r="L32" s="15">
+        <v>237</v>
+      </c>
+      <c r="M32" s="9">
+        <v>265</v>
+      </c>
+      <c r="N32" s="8">
+        <v>138</v>
+      </c>
+      <c r="O32" s="12">
+        <v>74</v>
+      </c>
+      <c r="P32" s="12">
         <v>53.6</v>
       </c>
-      <c r="P32">
-        <f>O32-O31</f>
+      <c r="Q32" s="19">
+        <f>P32-P31</f>
         <v>20.980000000000004</v>
       </c>
-      <c r="Q32">
+      <c r="R32" s="21">
         <f>G32-G31</f>
         <v>20.950000000000003</v>
       </c>
-      <c r="R32" s="4">
-        <f t="shared" ref="R32:R33" si="0">ROUNDDOWN(250/((E32/F32)*(D32/1000)),0)+(IF(L32&gt;L31,(L32-L31)/360,(L32+360-L31)/360))</f>
-        <v>33.050444444444445</v>
-      </c>
-      <c r="S32">
-        <f t="shared" ref="S32:S33" si="1">ROUNDDOWN(R32*(E32/F32),0)+IF(M32&gt;M31,(M32-M31)/360,(M32+360-M31)/360)</f>
-        <v>118.74444444444444</v>
-      </c>
-      <c r="T32">
-        <f t="shared" ref="T32:T33" si="2">S32*(D32/1000)</f>
-        <v>248.88835555555556</v>
-      </c>
-      <c r="U32">
-        <f t="shared" ref="U32:U33" si="3">H32-H31</f>
+      <c r="S32" s="22">
+        <f>ROUNDDOWN(250/((E32/F32)*(D32/1000)),0)+(IF(M32&gt;M31,(M32-M31)/360,(M32+360-M31)/360))</f>
+        <v>33.56111111111111</v>
+      </c>
+      <c r="T32" s="22">
+        <f>ROUNDDOWN(S32*(E32/F32),0)+IF(N32&gt;N31,(N32-N31)/360,(N32+360-N31)/360)</f>
+        <v>119.72777777777777</v>
+      </c>
+      <c r="U32" s="22">
+        <f>T32*(D32/1000)</f>
+        <v>250.94942222222224</v>
+      </c>
+      <c r="V32" s="21">
+        <f>H32-H31</f>
         <v>250.68999999999994</v>
       </c>
-      <c r="V32">
-        <f t="shared" ref="V32:V34" si="4">T32/P32</f>
-        <v>11.863124668996926</v>
-      </c>
-      <c r="W32">
-        <f t="shared" ref="W32:W38" si="5">R32*(E31/F31)*(D31/1000)</f>
-        <v>247.40618412698416</v>
-      </c>
-    </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="W32" s="22">
+        <f>S32*(E31/F31)*(D31/1000)</f>
+        <v>251.22888888888892</v>
+      </c>
+      <c r="X32" s="22">
+        <f t="shared" ref="X32:X34" si="0">U32/Q32</f>
+        <v>11.961364262260352</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B33">
         <v>10</v>
@@ -2064,60 +2545,64 @@
       <c r="H33">
         <v>1250.69</v>
       </c>
-      <c r="I33" s="6">
+      <c r="I33" s="4">
         <v>107.825</v>
       </c>
-      <c r="K33" s="2">
+      <c r="K33" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE(Videos_Folder,"\",A33,"-Lap",TEXT(B33,"00"),".MOV"),CONCATENATE(A33,"-Lap",TEXT(B33,"00"),".MOV"))</f>
+        <v>R07-Lap10.MOV</v>
+      </c>
+      <c r="L33" s="15">
         <v>231</v>
       </c>
-      <c r="L33" s="3">
-        <v>107.825</v>
-      </c>
-      <c r="M33">
+      <c r="M33" s="9">
+        <v>100</v>
+      </c>
+      <c r="N33" s="8">
         <v>8</v>
       </c>
-      <c r="N33">
+      <c r="O33" s="12">
         <v>352</v>
       </c>
-      <c r="O33">
+      <c r="P33" s="12">
         <v>74.97</v>
       </c>
-      <c r="P33">
-        <f>O33-O32</f>
+      <c r="Q33" s="19">
+        <f>P33-P32</f>
         <v>21.369999999999997</v>
       </c>
-      <c r="Q33">
+      <c r="R33" s="21">
         <f>G33-G32</f>
         <v>21.5</v>
       </c>
-      <c r="R33" s="4">
+      <c r="S33" s="22">
+        <f>ROUNDDOWN(250/((E33/F33)*(D33/1000)),0)+(IF(M33&gt;M32,(M33-M32)/360,(M33+360-M32)/360))</f>
+        <v>33.541666666666664</v>
+      </c>
+      <c r="T33" s="22">
+        <f>ROUNDDOWN(S33*(E33/F33),0)+IF(N33&gt;N32,(N33-N32)/360,(N33+360-N32)/360)</f>
+        <v>119.63888888888889</v>
+      </c>
+      <c r="U33" s="22">
+        <f>T33*(D33/1000)</f>
+        <v>250.7631111111111</v>
+      </c>
+      <c r="V33" s="21">
+        <f>H33-H32</f>
+        <v>252.2700000000001</v>
+      </c>
+      <c r="W33" s="22">
+        <f>S33*(E32/F32)*(D32/1000)</f>
+        <v>251.08333333333334</v>
+      </c>
+      <c r="X33" s="22">
         <f t="shared" si="0"/>
-        <v>33.74377777777778</v>
-      </c>
-      <c r="S33">
-        <f t="shared" si="1"/>
-        <v>120.62222222222222</v>
-      </c>
-      <c r="T33">
-        <f t="shared" si="2"/>
-        <v>252.82417777777778</v>
-      </c>
-      <c r="U33">
-        <f t="shared" si="3"/>
-        <v>252.2700000000001</v>
-      </c>
-      <c r="V33">
-        <f t="shared" si="4"/>
-        <v>11.830799147298915</v>
-      </c>
-      <c r="W33">
-        <f t="shared" si="5"/>
-        <v>252.5962793650794</v>
-      </c>
-    </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.35">
+        <v>11.734352415119847</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B34">
         <v>12</v>
@@ -2140,60 +2625,64 @@
       <c r="H34">
         <v>1500.885</v>
       </c>
-      <c r="I34" s="6">
+      <c r="I34" s="4">
         <v>275.93</v>
       </c>
-      <c r="K34" s="2">
+      <c r="K34" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE(Videos_Folder,"\",A34,"-Lap",TEXT(B34,"00"),".MOV"),CONCATENATE(A34,"-Lap",TEXT(B34,"00"),".MOV"))</f>
+        <v>R07-Lap12.MOV</v>
+      </c>
+      <c r="L34" s="15">
         <v>360</v>
       </c>
-      <c r="L34" s="3">
-        <v>275.93</v>
-      </c>
-      <c r="M34">
+      <c r="M34" s="9">
+        <v>270</v>
+      </c>
+      <c r="N34" s="8">
         <v>160</v>
       </c>
-      <c r="N34">
+      <c r="O34" s="12">
         <v>204</v>
       </c>
-      <c r="O34">
+      <c r="P34" s="12">
         <v>96.88</v>
       </c>
-      <c r="P34">
-        <f>O34-O33</f>
+      <c r="Q34" s="19">
+        <f>P34-P33</f>
         <v>21.909999999999997</v>
       </c>
-      <c r="Q34">
+      <c r="R34" s="21">
         <f>G34-G33</f>
         <v>21.909999999999997</v>
       </c>
-      <c r="R34" s="4">
-        <f t="shared" ref="R34" si="6">ROUNDDOWN(250/((E34/F34)*(D34/1000)),0)+(IF(L34&gt;L33,(L34-L33)/360,(L34+360-L33)/360))</f>
-        <v>33.466958333333331</v>
-      </c>
-      <c r="S34">
-        <f t="shared" ref="S34" si="7">ROUNDDOWN(R34*(E34/F34),0)+IF(M34&gt;M33,(M34-M33)/360,(M34+360-M33)/360)</f>
+      <c r="S34" s="22">
+        <f>ROUNDDOWN(250/((E34/F34)*(D34/1000)),0)+(IF(M34&gt;M33,(M34-M33)/360,(M34+360-M33)/360))</f>
+        <v>33.472222222222221</v>
+      </c>
+      <c r="T34" s="22">
+        <f>ROUNDDOWN(S34*(E34/F34),0)+IF(N34&gt;N33,(N34-N33)/360,(N34+360-N33)/360)</f>
         <v>119.42222222222222</v>
       </c>
-      <c r="T34">
-        <f t="shared" ref="T34" si="8">S34*(D34/1000)</f>
+      <c r="U34" s="22">
+        <f>T34*(D34/1000)</f>
         <v>250.30897777777778</v>
       </c>
-      <c r="U34">
-        <f t="shared" ref="U34" si="9">H34-H33</f>
+      <c r="V34" s="21">
+        <f>H34-H33</f>
         <v>250.19499999999994</v>
       </c>
-      <c r="V34">
-        <f t="shared" si="4"/>
+      <c r="W34" s="22">
+        <f>S34*(E33/F33)*(D33/1000)</f>
+        <v>250.56349206349208</v>
+      </c>
+      <c r="X34" s="22">
+        <f t="shared" si="0"/>
         <v>11.424417059688627</v>
       </c>
-      <c r="W34">
-        <f t="shared" si="5"/>
-        <v>250.52408809523808</v>
-      </c>
-    </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.35">
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B35">
         <v>14</v>
@@ -2216,60 +2705,64 @@
       <c r="H35">
         <v>1749.69</v>
       </c>
-      <c r="I35" s="6">
+      <c r="I35" s="4">
         <v>18.309999999999999</v>
       </c>
-      <c r="K35" s="2">
+      <c r="K35" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE(Videos_Folder,"\",A35,"-Lap",TEXT(B35,"00"),".MOV"),CONCATENATE(A35,"-Lap",TEXT(B35,"00"),".MOV"))</f>
+        <v>R07-Lap14.MOV</v>
+      </c>
+      <c r="L35" s="15">
         <v>357</v>
       </c>
-      <c r="L35" s="3">
-        <v>18.309999999999999</v>
-      </c>
-      <c r="M35">
+      <c r="M35" s="9">
+        <v>85</v>
+      </c>
+      <c r="N35" s="8">
         <v>286</v>
       </c>
-      <c r="N35">
+      <c r="O35" s="12">
         <v>40</v>
       </c>
-      <c r="O35">
+      <c r="P35" s="12">
         <v>119.23</v>
       </c>
-      <c r="P35">
-        <f>O35-O34</f>
+      <c r="Q35" s="19">
+        <f>P35-P34</f>
         <v>22.350000000000009</v>
       </c>
-      <c r="Q35">
+      <c r="R35" s="21">
         <f>G35-G34</f>
         <v>22.224999999999994</v>
       </c>
-      <c r="R35" s="4">
-        <f t="shared" ref="R35" si="10">ROUNDDOWN(250/((E35/F35)*(D35/1000)),0)+(IF(L35&gt;L34,(L35-L34)/360,(L35+360-L34)/360))</f>
-        <v>33.284388888888891</v>
-      </c>
-      <c r="S35">
-        <f t="shared" ref="S35" si="11">ROUNDDOWN(R35*(E35/F35),0)+IF(M35&gt;M34,(M35-M34)/360,(M35+360-M34)/360)</f>
-        <v>118.35</v>
-      </c>
-      <c r="T35">
-        <f t="shared" ref="T35" si="12">S35*(D35/1000)</f>
-        <v>248.0616</v>
-      </c>
-      <c r="U35">
+      <c r="S35" s="22">
+        <f>ROUNDDOWN(250/((E35/F35)*(D35/1000)),0)+(IF(M35&gt;M34,(M35-M34)/360,(M35+360-M34)/360))</f>
+        <v>33.486111111111114</v>
+      </c>
+      <c r="T35" s="22">
+        <f>ROUNDDOWN(S35*(E35/F35),0)+IF(N35&gt;N34,(N35-N34)/360,(N35+360-N34)/360)</f>
+        <v>119.35</v>
+      </c>
+      <c r="U35" s="22">
+        <f>T35*(D35/1000)</f>
+        <v>250.1576</v>
+      </c>
+      <c r="V35" s="21">
         <f>H35-H34</f>
         <v>248.80500000000006</v>
       </c>
-      <c r="V35">
-        <f t="shared" ref="V35" si="13">T35/P35</f>
-        <v>11.098953020134223</v>
-      </c>
-      <c r="W35">
-        <f t="shared" si="5"/>
-        <v>249.15742539682543</v>
-      </c>
-    </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="W35" s="22">
+        <f>S35*(E34/F34)*(D34/1000)</f>
+        <v>250.66746031746038</v>
+      </c>
+      <c r="X35" s="22">
+        <f t="shared" ref="X35" si="1">U35/Q35</f>
+        <v>11.192733780760623</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B36">
         <v>16</v>
@@ -2292,60 +2785,64 @@
       <c r="H36">
         <v>1999.5349999999901</v>
       </c>
-      <c r="I36" s="6">
+      <c r="I36" s="4">
         <v>168.99</v>
       </c>
-      <c r="K36" s="2">
+      <c r="K36" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE(Videos_Folder,"\",A36,"-Lap",TEXT(B36,"00"),".MOV"),CONCATENATE(A36,"-Lap",TEXT(B36,"00"),".MOV"))</f>
+        <v>R07-Lap16.MOV</v>
+      </c>
+      <c r="L36" s="15">
         <v>330</v>
       </c>
-      <c r="L36" s="3">
-        <v>168.99</v>
-      </c>
-      <c r="M36">
+      <c r="M36" s="9">
+        <v>247</v>
+      </c>
+      <c r="N36" s="8">
         <v>36</v>
       </c>
-      <c r="N36">
+      <c r="O36" s="12">
         <v>204</v>
       </c>
-      <c r="O36">
+      <c r="P36" s="12">
         <v>141.72</v>
       </c>
-      <c r="P36">
-        <f t="shared" ref="P36:P38" si="14">O36-O35</f>
+      <c r="Q36" s="19">
+        <f t="shared" ref="Q36:Q38" si="2">P36-P35</f>
         <v>22.489999999999995</v>
       </c>
-      <c r="Q36">
-        <f t="shared" ref="Q36:Q38" si="15">G36-G35</f>
+      <c r="R36" s="21">
+        <f>G36-G35</f>
         <v>22.455000000000013</v>
       </c>
-      <c r="R36" s="4">
-        <f t="shared" ref="R36:R38" si="16">ROUNDDOWN(250/((E36/F36)*(D36/1000)),0)+(IF(L36&gt;L35,(L36-L35)/360,(L36+360-L35)/360))</f>
-        <v>33.418555555555557</v>
-      </c>
-      <c r="S36">
-        <f t="shared" ref="S36:S38" si="17">ROUNDDOWN(R36*(E36/F36),0)+IF(M36&gt;M35,(M36-M35)/360,(M36+360-M35)/360)</f>
+      <c r="S36" s="22">
+        <f>ROUNDDOWN(250/((E36/F36)*(D36/1000)),0)+(IF(M36&gt;M35,(M36-M35)/360,(M36+360-M35)/360))</f>
+        <v>33.450000000000003</v>
+      </c>
+      <c r="T36" s="22">
+        <f>ROUNDDOWN(S36*(E36/F36),0)+IF(N36&gt;N35,(N36-N35)/360,(N36+360-N35)/360)</f>
         <v>119.30555555555556</v>
       </c>
-      <c r="T36">
-        <f t="shared" ref="T36:T38" si="18">S36*(D36/1000)</f>
+      <c r="U36" s="22">
+        <f>T36*(D36/1000)</f>
         <v>250.06444444444446</v>
       </c>
-      <c r="U36">
-        <f t="shared" ref="U36:U38" si="19">H36-H35</f>
+      <c r="V36" s="21">
+        <f>H36-H35</f>
         <v>249.84499999999002</v>
       </c>
-      <c r="V36">
-        <f t="shared" ref="V36:V38" si="20">T36/P36</f>
+      <c r="W36" s="22">
+        <f>S36*(E35/F35)*(D35/1000)</f>
+        <v>250.39714285714291</v>
+      </c>
+      <c r="X36" s="22">
+        <f t="shared" ref="X36:X38" si="3">U36/Q36</f>
         <v>11.118917049552891</v>
       </c>
-      <c r="W36">
-        <f t="shared" si="5"/>
-        <v>250.16175873015877</v>
-      </c>
-    </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.35">
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B37">
         <v>18</v>
@@ -2368,60 +2865,64 @@
       <c r="H37">
         <v>2250.5949999999998</v>
       </c>
-      <c r="I37" s="6">
+      <c r="I37" s="4">
         <v>20.03</v>
       </c>
-      <c r="K37" s="2">
+      <c r="K37" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE(Videos_Folder,"\",A37,"-Lap",TEXT(B37,"00"),".MOV"),CONCATENATE(A37,"-Lap",TEXT(B37,"00"),".MOV"))</f>
+        <v>R07-Lap18.MOV</v>
+      </c>
+      <c r="L37" s="15">
         <v>707</v>
       </c>
-      <c r="L37" s="3">
-        <v>20.03</v>
-      </c>
-      <c r="M37">
+      <c r="M37" s="9">
+        <v>57</v>
+      </c>
+      <c r="N37" s="8">
         <v>190</v>
       </c>
-      <c r="N37">
+      <c r="O37" s="12">
         <v>56</v>
       </c>
-      <c r="O37">
+      <c r="P37" s="12">
         <v>164.21</v>
       </c>
-      <c r="P37">
-        <f t="shared" si="14"/>
+      <c r="Q37" s="19">
+        <f t="shared" si="2"/>
         <v>22.490000000000009</v>
       </c>
-      <c r="Q37">
-        <f t="shared" si="15"/>
+      <c r="R37" s="21">
+        <f>G37-G36</f>
         <v>22.569999999999993</v>
       </c>
-      <c r="R37" s="4">
-        <f t="shared" si="16"/>
-        <v>33.586222222222219</v>
-      </c>
-      <c r="S37">
-        <f t="shared" si="17"/>
+      <c r="S37" s="22">
+        <f>ROUNDDOWN(250/((E37/F37)*(D37/1000)),0)+(IF(M37&gt;M36,(M37-M36)/360,(M37+360-M36)/360))</f>
+        <v>33.472222222222221</v>
+      </c>
+      <c r="T37" s="22">
+        <f>ROUNDDOWN(S37*(E37/F37),0)+IF(N37&gt;N36,(N37-N36)/360,(N37+360-N36)/360)</f>
         <v>119.42777777777778</v>
       </c>
-      <c r="T37">
-        <f t="shared" si="18"/>
+      <c r="U37" s="22">
+        <f>T37*(D37/1000)</f>
         <v>250.32062222222223</v>
       </c>
-      <c r="U37">
-        <f t="shared" si="19"/>
+      <c r="V37" s="21">
+        <f>H37-H36</f>
         <v>251.06000000000972</v>
       </c>
-      <c r="V37">
-        <f t="shared" si="20"/>
+      <c r="W37" s="22">
+        <f>S37*(E36/F36)*(D36/1000)</f>
+        <v>250.56349206349208</v>
+      </c>
+      <c r="X37" s="22">
+        <f t="shared" si="3"/>
         <v>11.130307791117035</v>
       </c>
-      <c r="W37">
-        <f t="shared" si="5"/>
-        <v>251.41686349206347</v>
-      </c>
-    </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.35">
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B38">
         <v>20</v>
@@ -2444,240 +2945,311 @@
       <c r="H38">
         <v>2501.0549999999998</v>
       </c>
-      <c r="I38" s="6">
+      <c r="I38" s="4">
         <v>108.655</v>
       </c>
-      <c r="K38" s="2">
+      <c r="K38" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE(Videos_Folder,"\",A38,"-Lap",TEXT(B38,"00"),".MOV"),CONCATENATE(A38,"-Lap",TEXT(B38,"00"),".MOV"))</f>
+        <v>R07-Lap20.MOV</v>
+      </c>
+      <c r="L38" s="15">
         <v>456</v>
       </c>
-      <c r="L38" s="3">
-        <v>108.655</v>
-      </c>
-      <c r="M38">
+      <c r="M38" s="9">
+        <v>115</v>
+      </c>
+      <c r="N38" s="8">
         <v>265</v>
       </c>
-      <c r="N38">
+      <c r="O38" s="12">
         <v>184</v>
       </c>
-      <c r="O38">
+      <c r="P38" s="12">
         <v>186.84</v>
       </c>
-      <c r="P38">
-        <f t="shared" si="14"/>
+      <c r="Q38" s="19">
+        <f t="shared" si="2"/>
         <v>22.629999999999995</v>
       </c>
-      <c r="Q38">
-        <f t="shared" si="15"/>
+      <c r="R38" s="21">
+        <f>G38-G37</f>
         <v>22.689999999999998</v>
       </c>
-      <c r="R38" s="4">
-        <f t="shared" si="16"/>
-        <v>35.246180555555554</v>
-      </c>
-      <c r="S38">
-        <f t="shared" si="17"/>
+      <c r="S38" s="22">
+        <f>ROUNDDOWN(250/((E38/F38)*(D38/1000)),0)+(IF(M38&gt;M37,(M38-M37)/360,(M38+360-M37)/360))</f>
+        <v>35.161111111111111</v>
+      </c>
+      <c r="T38" s="22">
+        <f>ROUNDDOWN(S38*(E38/F38),0)+IF(N38&gt;N37,(N38-N37)/360,(N38+360-N37)/360)</f>
         <v>117.20833333333333</v>
       </c>
-      <c r="T38">
-        <f t="shared" si="18"/>
+      <c r="U38" s="22">
+        <f>T38*(D38/1000)</f>
         <v>245.66866666666667</v>
       </c>
-      <c r="U38">
-        <f t="shared" si="19"/>
+      <c r="V38" s="21">
+        <f>H38-H37</f>
         <v>250.46000000000004</v>
       </c>
-      <c r="V38">
-        <f t="shared" si="20"/>
+      <c r="W38" s="22">
+        <f>S38*(E37/F37)*(D37/1000)</f>
+        <v>263.20603174603178</v>
+      </c>
+      <c r="X38" s="22">
+        <f t="shared" si="3"/>
         <v>10.855884519074976</v>
       </c>
-      <c r="W38">
-        <f t="shared" si="5"/>
-        <v>263.84283730158728</v>
-      </c>
-      <c r="X38" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>10</v>
-      </c>
-      <c r="B39">
+      <c r="Y38" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" s="7">
         <v>20</v>
       </c>
-      <c r="C39">
-        <v>0</v>
-      </c>
-      <c r="D39">
-        <v>0</v>
-      </c>
-      <c r="E39">
-        <v>0</v>
-      </c>
-      <c r="F39">
-        <v>0</v>
-      </c>
-      <c r="G39">
-        <v>0</v>
-      </c>
-      <c r="H39">
-        <v>0</v>
-      </c>
-      <c r="I39">
-        <v>11.393987039562001</v>
-      </c>
-      <c r="P39">
-        <f>O38-O30</f>
+      <c r="C39" s="7">
+        <v>0</v>
+      </c>
+      <c r="D39" s="7">
+        <v>0</v>
+      </c>
+      <c r="E39" s="7">
+        <v>0</v>
+      </c>
+      <c r="F39" s="7">
+        <v>0</v>
+      </c>
+      <c r="G39" s="7">
+        <v>0</v>
+      </c>
+      <c r="H39" s="7">
+        <v>11.2814562281121</v>
+      </c>
+      <c r="I39" s="7">
+        <v>0</v>
+      </c>
+      <c r="J39" s="13"/>
+      <c r="K39" s="16"/>
+      <c r="L39" s="16"/>
+      <c r="M39" s="9"/>
+      <c r="N39" s="8"/>
+      <c r="O39" s="8"/>
+      <c r="P39" s="8"/>
+      <c r="Q39" s="2">
+        <f>P38-P30</f>
         <v>175.88</v>
       </c>
-      <c r="Q39">
+      <c r="R39" s="20">
         <f>G38-G30</f>
         <v>175.91499999999999</v>
       </c>
-      <c r="R39" s="4">
-        <f>ROUNDDOWN(2000/((E38/F38)*(D38/1000)),0)+(IF(L38&gt;L30,(L38-L30)/360,(L38+360-L30)/360))</f>
-        <v>286.854625</v>
-      </c>
-      <c r="S39">
-        <f>ROUNDDOWN(R39*(E38/F38),0)+IF(M38&gt;M30,(M38-M30)/360,(M38+360-M30)/360)</f>
-        <v>956.91944444444448</v>
-      </c>
-      <c r="T39">
-        <f>S39*(D38/1000)</f>
-        <v>2005.7031555555557</v>
-      </c>
-      <c r="U39">
+      <c r="S39" s="5">
+        <f>ROUNDDOWN(2000/((E38/F38)*(D38/1000)),0)+(IF(M38&gt;M30,(M38-M30)/360,(M38+360-M30)/360))</f>
+        <v>286.77777777777777</v>
+      </c>
+      <c r="T39" s="5">
+        <f>ROUNDDOWN(S39*(E38/F38),0)+IF(N38&gt;N30,(N38-N30)/360,(N38+360-N30)/360)</f>
+        <v>955.91944444444448</v>
+      </c>
+      <c r="U39" s="5">
+        <f>T39*(D38/1000)</f>
+        <v>2003.6071555555557</v>
+      </c>
+      <c r="V39" s="23">
         <f>H38-H30</f>
         <v>2004.0749999999998</v>
       </c>
-    </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+      <c r="W39" s="5"/>
+      <c r="X39" s="5"/>
+    </row>
+    <row r="40" spans="1:25" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" s="7">
+        <v>20</v>
+      </c>
+      <c r="C40" s="7">
+        <v>0</v>
+      </c>
+      <c r="D40" s="7">
+        <v>0</v>
+      </c>
+      <c r="E40" s="7">
+        <v>0</v>
+      </c>
+      <c r="F40" s="7">
+        <v>0</v>
+      </c>
+      <c r="G40" s="7">
+        <v>0</v>
+      </c>
+      <c r="H40" s="7">
+        <v>11.5330050025012</v>
+      </c>
+      <c r="I40" s="7">
+        <v>0</v>
+      </c>
+      <c r="J40" s="13"/>
+      <c r="K40" s="16"/>
+      <c r="L40" s="16"/>
+      <c r="M40" s="9"/>
+      <c r="N40" s="8"/>
+      <c r="O40" s="8"/>
+      <c r="P40" s="8"/>
+      <c r="Q40" s="2"/>
+      <c r="R40" s="20"/>
+      <c r="S40" s="5"/>
+      <c r="T40" s="5"/>
+      <c r="U40" s="5">
+        <f>U39/Q39</f>
+        <v>11.39189876936295</v>
+      </c>
+      <c r="V40" s="23">
+        <f>V39/R39</f>
+        <v>11.39229173180229</v>
+      </c>
+      <c r="W40" s="5"/>
+      <c r="X40" s="5"/>
+    </row>
+    <row r="41" spans="1:25" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B40">
+      <c r="B41" s="7">
         <v>20</v>
       </c>
-      <c r="C40">
-        <v>0</v>
-      </c>
-      <c r="D40">
-        <v>0</v>
-      </c>
-      <c r="E40">
-        <v>0</v>
-      </c>
-      <c r="F40">
-        <v>0</v>
-      </c>
-      <c r="G40">
-        <v>0</v>
-      </c>
-      <c r="H40">
-        <v>0</v>
-      </c>
-      <c r="I40">
-        <v>11.6359510004547</v>
-      </c>
-      <c r="T40">
-        <f>T39/P39</f>
-        <v>11.40381598564678</v>
-      </c>
-      <c r="U40">
-        <f>U39/Q39</f>
-        <v>11.39229173180229</v>
-      </c>
-    </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
+      <c r="C41" s="7">
+        <v>0</v>
+      </c>
+      <c r="D41" s="7">
+        <v>0</v>
+      </c>
+      <c r="E41" s="7">
+        <v>0</v>
+      </c>
+      <c r="F41" s="7">
+        <v>0</v>
+      </c>
+      <c r="G41" s="7">
+        <v>0</v>
+      </c>
+      <c r="H41" s="7">
+        <v>11.318063678042099</v>
+      </c>
+      <c r="I41" s="7">
+        <v>0</v>
+      </c>
+      <c r="J41" s="13"/>
+      <c r="K41" s="16"/>
+      <c r="L41" s="16"/>
+      <c r="M41" s="9"/>
+      <c r="N41" s="8"/>
+      <c r="O41" s="8"/>
+      <c r="P41" s="8"/>
+      <c r="Q41" s="2"/>
+      <c r="R41" s="20"/>
+      <c r="S41" s="5"/>
+      <c r="T41" s="5"/>
+      <c r="U41" s="5"/>
+      <c r="V41" s="23"/>
+      <c r="W41" s="5"/>
+      <c r="X41" s="5"/>
+    </row>
+    <row r="42" spans="1:25" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B41">
+      <c r="B42" s="7">
         <v>20</v>
       </c>
-      <c r="C41">
-        <v>0</v>
-      </c>
-      <c r="D41">
-        <v>0</v>
-      </c>
-      <c r="E41">
-        <v>0</v>
-      </c>
-      <c r="F41">
-        <v>0</v>
-      </c>
-      <c r="G41">
-        <v>0</v>
-      </c>
-      <c r="H41">
-        <v>0</v>
-      </c>
-      <c r="I41">
-        <v>11.395747783082101</v>
-      </c>
-    </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+      <c r="C42" s="7">
+        <v>0</v>
+      </c>
+      <c r="D42" s="7">
+        <v>0</v>
+      </c>
+      <c r="E42" s="7">
+        <v>0</v>
+      </c>
+      <c r="F42" s="7">
+        <v>0</v>
+      </c>
+      <c r="G42" s="7">
+        <v>0</v>
+      </c>
+      <c r="H42" s="7">
+        <v>11.554790654110899</v>
+      </c>
+      <c r="I42" s="7">
+        <v>0</v>
+      </c>
+      <c r="J42" s="13"/>
+      <c r="K42" s="16"/>
+      <c r="L42" s="16"/>
+      <c r="M42" s="9"/>
+      <c r="N42" s="8"/>
+      <c r="O42" s="8"/>
+      <c r="P42" s="8"/>
+      <c r="Q42" s="2"/>
+      <c r="R42" s="20"/>
+      <c r="S42" s="2"/>
+      <c r="T42" s="2"/>
+      <c r="U42" s="2"/>
+      <c r="V42" s="20"/>
+      <c r="W42" s="2"/>
+      <c r="X42" s="2"/>
+    </row>
+    <row r="43" spans="1:25" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B42">
+      <c r="B43" s="7">
         <v>20</v>
       </c>
-      <c r="C42">
-        <v>0</v>
-      </c>
-      <c r="D42">
-        <v>0</v>
-      </c>
-      <c r="E42">
-        <v>0</v>
-      </c>
-      <c r="F42">
-        <v>0</v>
-      </c>
-      <c r="G42">
-        <v>0</v>
-      </c>
-      <c r="H42">
-        <v>0</v>
-      </c>
-      <c r="I42">
-        <v>11.6359188835834</v>
-      </c>
-    </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>14</v>
-      </c>
-      <c r="B43">
+      <c r="C43" s="7">
+        <v>0</v>
+      </c>
+      <c r="D43" s="7">
+        <v>0</v>
+      </c>
+      <c r="E43" s="7">
+        <v>0</v>
+      </c>
+      <c r="F43" s="7">
+        <v>0</v>
+      </c>
+      <c r="G43" s="7">
+        <v>0</v>
+      </c>
+      <c r="H43" s="7">
+        <v>11.3308485642397</v>
+      </c>
+      <c r="I43" s="7">
+        <v>0</v>
+      </c>
+      <c r="J43" s="13"/>
+      <c r="K43" s="16"/>
+      <c r="L43" s="16"/>
+      <c r="M43" s="9"/>
+      <c r="N43" s="8"/>
+      <c r="O43" s="8"/>
+      <c r="P43" s="8"/>
+      <c r="Q43" s="2"/>
+      <c r="R43" s="20"/>
+      <c r="S43" s="2"/>
+      <c r="T43" s="2"/>
+      <c r="U43" s="2"/>
+      <c r="V43" s="20"/>
+      <c r="W43" s="2"/>
+      <c r="X43" s="2"/>
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>20</v>
-      </c>
-      <c r="C43">
-        <v>0</v>
-      </c>
-      <c r="D43">
-        <v>0</v>
-      </c>
-      <c r="E43">
-        <v>0</v>
-      </c>
-      <c r="F43">
-        <v>0</v>
-      </c>
-      <c r="G43">
-        <v>0</v>
-      </c>
-      <c r="H43">
-        <v>0</v>
-      </c>
-      <c r="I43">
-        <v>11.408769487965101</v>
-      </c>
-    </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>17</v>
       </c>
       <c r="B44">
         <v>4</v>
@@ -2703,36 +3275,26 @@
       <c r="I44">
         <v>146.67500000000001</v>
       </c>
-      <c r="L44" s="3">
+      <c r="K44" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE(Videos_Folder,"\",A44,"-Lap",TEXT(B44,"00"),".MOV"),CONCATENATE(A44,"-Lap",TEXT(B44,"00"),".MOV"))</f>
+        <v>R08-Lap04.MOV</v>
+      </c>
+      <c r="M44" s="9">
         <v>180</v>
       </c>
-      <c r="M44">
+      <c r="N44" s="8">
         <v>190</v>
       </c>
-      <c r="N44">
+      <c r="O44" s="12">
         <v>10</v>
       </c>
-      <c r="O44">
+      <c r="P44" s="12">
         <v>12.37</v>
       </c>
-      <c r="Q44">
-        <v>195</v>
-      </c>
-      <c r="R44">
-        <v>294</v>
-      </c>
-      <c r="T44">
-        <f>IF(Q44+180&gt;360,Q44-180,Q44+180)</f>
-        <v>15</v>
-      </c>
-      <c r="U44">
-        <f t="shared" ref="U44:U52" si="21">IF(R44+180&gt;360,R44-180,R44+180)</f>
-        <v>114</v>
-      </c>
-    </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.35">
+    </row>
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B45">
         <v>6</v>
@@ -2758,24 +3320,15 @@
       <c r="I45">
         <v>115.13</v>
       </c>
-      <c r="Q45">
-        <v>48</v>
-      </c>
-      <c r="R45">
-        <v>236</v>
-      </c>
-      <c r="T45">
-        <f t="shared" ref="T45:T52" si="22">IF(Q45+180&gt;360,Q45-180,Q45+180)</f>
-        <v>228</v>
-      </c>
-      <c r="U45">
-        <f t="shared" si="21"/>
-        <v>56</v>
-      </c>
-    </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="K45" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE(Videos_Folder,"\",A45,"-Lap",TEXT(B45,"00"),".MOV"),CONCATENATE(A45,"-Lap",TEXT(B45,"00"),".MOV"))</f>
+        <v>R08-Lap06.MOV</v>
+      </c>
+      <c r="M45" s="9"/>
+    </row>
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B46">
         <v>8</v>
@@ -2801,24 +3354,15 @@
       <c r="I46">
         <v>126.2</v>
       </c>
-      <c r="Q46">
-        <v>260</v>
-      </c>
-      <c r="R46">
-        <v>144</v>
-      </c>
-      <c r="T46">
-        <f t="shared" si="22"/>
-        <v>80</v>
-      </c>
-      <c r="U46">
-        <f t="shared" si="21"/>
-        <v>324</v>
-      </c>
-    </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="K46" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE(Videos_Folder,"\",A46,"-Lap",TEXT(B46,"00"),".MOV"),CONCATENATE(A46,"-Lap",TEXT(B46,"00"),".MOV"))</f>
+        <v>R08-Lap08.MOV</v>
+      </c>
+      <c r="M46" s="9"/>
+    </row>
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B47">
         <v>10</v>
@@ -2844,24 +3388,15 @@
       <c r="I47">
         <v>178.63</v>
       </c>
-      <c r="Q47">
-        <v>100</v>
-      </c>
-      <c r="R47">
-        <v>8</v>
-      </c>
-      <c r="T47">
-        <f t="shared" si="22"/>
-        <v>280</v>
-      </c>
-      <c r="U47">
-        <f t="shared" si="21"/>
-        <v>188</v>
-      </c>
-    </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="K47" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE(Videos_Folder,"\",A47,"-Lap",TEXT(B47,"00"),".MOV"),CONCATENATE(A47,"-Lap",TEXT(B47,"00"),".MOV"))</f>
+        <v>R08-Lap10.MOV</v>
+      </c>
+      <c r="M47" s="9"/>
+    </row>
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B48">
         <v>12</v>
@@ -2887,24 +3422,15 @@
       <c r="I48">
         <v>124.79</v>
       </c>
-      <c r="Q48">
-        <v>270</v>
-      </c>
-      <c r="R48">
-        <v>160</v>
-      </c>
-      <c r="T48">
-        <f t="shared" si="22"/>
-        <v>90</v>
-      </c>
-      <c r="U48">
-        <f t="shared" si="21"/>
-        <v>340</v>
-      </c>
-    </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="K48" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE(Videos_Folder,"\",A48,"-Lap",TEXT(B48,"00"),".MOV"),CONCATENATE(A48,"-Lap",TEXT(B48,"00"),".MOV"))</f>
+        <v>R08-Lap12.MOV</v>
+      </c>
+      <c r="M48" s="9"/>
+    </row>
+    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B49">
         <v>14</v>
@@ -2930,24 +3456,15 @@
       <c r="I49">
         <v>145.88</v>
       </c>
-      <c r="Q49">
-        <v>85</v>
-      </c>
-      <c r="R49">
-        <v>286</v>
-      </c>
-      <c r="T49">
-        <f t="shared" si="22"/>
-        <v>265</v>
-      </c>
-      <c r="U49">
-        <f t="shared" si="21"/>
-        <v>106</v>
-      </c>
-    </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="K49" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE(Videos_Folder,"\",A49,"-Lap",TEXT(B49,"00"),".MOV"),CONCATENATE(A49,"-Lap",TEXT(B49,"00"),".MOV"))</f>
+        <v>R08-Lap14.MOV</v>
+      </c>
+      <c r="M49" s="9"/>
+    </row>
+    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B50">
         <v>16</v>
@@ -2973,24 +3490,15 @@
       <c r="I50">
         <v>219.53</v>
       </c>
-      <c r="Q50">
-        <v>247</v>
-      </c>
-      <c r="R50">
-        <v>36</v>
-      </c>
-      <c r="T50">
-        <f t="shared" si="22"/>
-        <v>67</v>
-      </c>
-      <c r="U50">
-        <f t="shared" si="21"/>
-        <v>216</v>
-      </c>
-    </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="K50" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE(Videos_Folder,"\",A50,"-Lap",TEXT(B50,"00"),".MOV"),CONCATENATE(A50,"-Lap",TEXT(B50,"00"),".MOV"))</f>
+        <v>R08-Lap16.MOV</v>
+      </c>
+      <c r="M50" s="9"/>
+    </row>
+    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B51">
         <v>18</v>
@@ -3016,24 +3524,15 @@
       <c r="I51">
         <v>147.33000000000001</v>
       </c>
-      <c r="Q51">
-        <v>57</v>
-      </c>
-      <c r="R51">
-        <v>190</v>
-      </c>
-      <c r="T51">
-        <f t="shared" si="22"/>
-        <v>237</v>
-      </c>
-      <c r="U51">
-        <f t="shared" si="21"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="K51" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE(Videos_Folder,"\",A51,"-Lap",TEXT(B51,"00"),".MOV"),CONCATENATE(A51,"-Lap",TEXT(B51,"00"),".MOV"))</f>
+        <v>R08-Lap18.MOV</v>
+      </c>
+      <c r="M51" s="9"/>
+    </row>
+    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B52">
         <v>20</v>
@@ -3059,165 +3558,231 @@
       <c r="I52">
         <v>183.76</v>
       </c>
-      <c r="Q52">
-        <v>115</v>
-      </c>
-      <c r="R52">
-        <v>265</v>
-      </c>
-      <c r="T52">
-        <f t="shared" si="22"/>
-        <v>295</v>
-      </c>
-      <c r="U52">
-        <f t="shared" si="21"/>
-        <v>85</v>
-      </c>
-    </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
+      <c r="K52" s="17" t="str">
+        <f>HYPERLINK(CONCATENATE(Videos_Folder,"\",A52,"-Lap",TEXT(B52,"00"),".MOV"),CONCATENATE(A52,"-Lap",TEXT(B52,"00"),".MOV"))</f>
+        <v>R08-Lap20.MOV</v>
+      </c>
+      <c r="M52" s="9"/>
+    </row>
+    <row r="53" spans="1:24" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B53" s="7">
+        <v>20</v>
+      </c>
+      <c r="C53" s="7">
+        <v>0</v>
+      </c>
+      <c r="D53" s="7">
+        <v>0</v>
+      </c>
+      <c r="E53" s="7">
+        <v>0</v>
+      </c>
+      <c r="F53" s="7">
+        <v>0</v>
+      </c>
+      <c r="G53" s="7">
+        <v>0</v>
+      </c>
+      <c r="H53" s="7">
+        <v>11.4576041719406</v>
+      </c>
+      <c r="I53" s="7">
+        <v>0</v>
+      </c>
+      <c r="J53" s="13"/>
+      <c r="K53" s="16"/>
+      <c r="L53" s="16"/>
+      <c r="M53" s="9"/>
+      <c r="N53" s="8"/>
+      <c r="O53" s="8"/>
+      <c r="P53" s="8"/>
+      <c r="Q53" s="2"/>
+      <c r="R53" s="20"/>
+      <c r="S53" s="2"/>
+      <c r="T53" s="2"/>
+      <c r="U53" s="2"/>
+      <c r="V53" s="20"/>
+      <c r="W53" s="2"/>
+      <c r="X53" s="2"/>
+    </row>
+    <row r="54" spans="1:24" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B53">
+      <c r="B54" s="7">
         <v>20</v>
       </c>
-      <c r="C53">
-        <v>0</v>
-      </c>
-      <c r="D53">
-        <v>0</v>
-      </c>
-      <c r="E53">
-        <v>0</v>
-      </c>
-      <c r="F53">
-        <v>0</v>
-      </c>
-      <c r="G53">
-        <v>0</v>
-      </c>
-      <c r="H53">
-        <v>0</v>
-      </c>
-      <c r="I53">
-        <v>11.5253697749199</v>
-      </c>
-    </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
+      <c r="C54" s="7">
+        <v>0</v>
+      </c>
+      <c r="D54" s="7">
+        <v>0</v>
+      </c>
+      <c r="E54" s="7">
+        <v>0</v>
+      </c>
+      <c r="F54" s="7">
+        <v>0</v>
+      </c>
+      <c r="G54" s="7">
+        <v>0</v>
+      </c>
+      <c r="H54" s="7">
+        <v>11.184527872006701</v>
+      </c>
+      <c r="I54" s="7">
+        <v>0</v>
+      </c>
+      <c r="J54" s="13"/>
+      <c r="K54" s="16"/>
+      <c r="L54" s="16"/>
+      <c r="M54" s="9"/>
+      <c r="N54" s="8"/>
+      <c r="O54" s="8"/>
+      <c r="P54" s="8"/>
+      <c r="Q54" s="2"/>
+      <c r="R54" s="20"/>
+      <c r="S54" s="2"/>
+      <c r="T54" s="2"/>
+      <c r="U54" s="2"/>
+      <c r="V54" s="20"/>
+      <c r="W54" s="2"/>
+      <c r="X54" s="2"/>
+    </row>
+    <row r="55" spans="1:24" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B54">
+      <c r="B55" s="7">
         <v>20</v>
       </c>
-      <c r="C54">
-        <v>0</v>
-      </c>
-      <c r="D54">
-        <v>0</v>
-      </c>
-      <c r="E54">
-        <v>0</v>
-      </c>
-      <c r="F54">
-        <v>0</v>
-      </c>
-      <c r="G54">
-        <v>0</v>
-      </c>
-      <c r="H54">
-        <v>0</v>
-      </c>
-      <c r="I54">
-        <v>11.247356453835801</v>
-      </c>
-    </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
+      <c r="C55" s="7">
+        <v>0</v>
+      </c>
+      <c r="D55" s="7">
+        <v>0</v>
+      </c>
+      <c r="E55" s="7">
+        <v>0</v>
+      </c>
+      <c r="F55" s="7">
+        <v>0</v>
+      </c>
+      <c r="G55" s="7">
+        <v>0</v>
+      </c>
+      <c r="H55" s="7">
+        <v>11.4711286537779</v>
+      </c>
+      <c r="I55" s="7">
+        <v>0</v>
+      </c>
+      <c r="J55" s="13"/>
+      <c r="K55" s="16"/>
+      <c r="L55" s="16"/>
+      <c r="M55" s="9"/>
+      <c r="N55" s="8"/>
+      <c r="O55" s="8"/>
+      <c r="P55" s="8"/>
+      <c r="Q55" s="2"/>
+      <c r="R55" s="20"/>
+      <c r="S55" s="2"/>
+      <c r="T55" s="2"/>
+      <c r="U55" s="2"/>
+      <c r="V55" s="20"/>
+      <c r="W55" s="2"/>
+      <c r="X55" s="2"/>
+    </row>
+    <row r="56" spans="1:24" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B55">
+      <c r="B56" s="7">
         <v>20</v>
       </c>
-      <c r="C55">
-        <v>0</v>
-      </c>
-      <c r="D55">
-        <v>0</v>
-      </c>
-      <c r="E55">
-        <v>0</v>
-      </c>
-      <c r="F55">
-        <v>0</v>
-      </c>
-      <c r="G55">
-        <v>0</v>
-      </c>
-      <c r="H55">
-        <v>0</v>
-      </c>
-      <c r="I55">
-        <v>11.5243327974284</v>
-      </c>
-    </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
+      <c r="C56" s="7">
+        <v>0</v>
+      </c>
+      <c r="D56" s="7">
+        <v>0</v>
+      </c>
+      <c r="E56" s="7">
+        <v>0</v>
+      </c>
+      <c r="F56" s="7">
+        <v>0</v>
+      </c>
+      <c r="G56" s="7">
+        <v>0</v>
+      </c>
+      <c r="H56" s="7">
+        <v>11.202569401762201</v>
+      </c>
+      <c r="I56" s="7">
+        <v>0</v>
+      </c>
+      <c r="J56" s="13"/>
+      <c r="K56" s="16"/>
+      <c r="L56" s="16"/>
+      <c r="M56" s="9"/>
+      <c r="N56" s="8"/>
+      <c r="O56" s="8"/>
+      <c r="P56" s="8"/>
+      <c r="Q56" s="2"/>
+      <c r="R56" s="20"/>
+      <c r="S56" s="2"/>
+      <c r="T56" s="2"/>
+      <c r="U56" s="2"/>
+      <c r="V56" s="20"/>
+      <c r="W56" s="2"/>
+      <c r="X56" s="2"/>
+    </row>
+    <row r="57" spans="1:24" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B56">
+      <c r="B57" s="7">
         <v>20</v>
       </c>
-      <c r="C56">
-        <v>0</v>
-      </c>
-      <c r="D56">
-        <v>0</v>
-      </c>
-      <c r="E56">
-        <v>0</v>
-      </c>
-      <c r="F56">
-        <v>0</v>
-      </c>
-      <c r="G56">
-        <v>0</v>
-      </c>
-      <c r="H56">
-        <v>0</v>
-      </c>
-      <c r="I56">
-        <v>11.2473056384936</v>
-      </c>
-    </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>14</v>
-      </c>
-      <c r="B57">
-        <v>20</v>
-      </c>
-      <c r="C57">
-        <v>0</v>
-      </c>
-      <c r="D57">
-        <v>0</v>
-      </c>
-      <c r="E57">
-        <v>0</v>
-      </c>
-      <c r="F57">
-        <v>0</v>
-      </c>
-      <c r="G57">
-        <v>0</v>
-      </c>
-      <c r="H57">
-        <v>0</v>
-      </c>
-      <c r="I57">
-        <v>11.538368479282701</v>
-      </c>
+      <c r="C57" s="7">
+        <v>0</v>
+      </c>
+      <c r="D57" s="7">
+        <v>0</v>
+      </c>
+      <c r="E57" s="7">
+        <v>0</v>
+      </c>
+      <c r="F57" s="7">
+        <v>0</v>
+      </c>
+      <c r="G57" s="7">
+        <v>0</v>
+      </c>
+      <c r="H57" s="7">
+        <v>11.482495480661701</v>
+      </c>
+      <c r="I57" s="7">
+        <v>0</v>
+      </c>
+      <c r="J57" s="13"/>
+      <c r="K57" s="16"/>
+      <c r="L57" s="16"/>
+      <c r="M57" s="9"/>
+      <c r="N57" s="8"/>
+      <c r="O57" s="8"/>
+      <c r="P57" s="8"/>
+      <c r="Q57" s="2"/>
+      <c r="R57" s="20"/>
+      <c r="S57" s="2"/>
+      <c r="T57" s="2"/>
+      <c r="U57" s="2"/>
+      <c r="V57" s="20"/>
+      <c r="W57" s="2"/>
+      <c r="X57" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>